<commit_message>
300: concepts show relevant properties for subject/object
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/process.xlsx
+++ b/documentation-generator/vocab_csv/process.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="264">
   <si>
     <t>preffix</t>
   </si>
@@ -631,7 +631,7 @@
     <t>Resolution</t>
   </si>
   <si>
-    <t>dpv:PersonalDataHandling</t>
+    <t>PersonalDataHandling</t>
   </si>
   <si>
     <t>Personal Data Handling</t>
@@ -676,103 +676,112 @@
     <t>Harshvardhan J. Pandit</t>
   </si>
   <si>
+    <t>PersonalDataProcess</t>
+  </si>
+  <si>
+    <t>Personal Data Process</t>
+  </si>
+  <si>
+    <t>An action, activity, or method involving personal data</t>
+  </si>
+  <si>
+    <t>NonPersonalDataProcess</t>
+  </si>
+  <si>
+    <t>Non-Personal Data Process</t>
+  </si>
+  <si>
+    <t>An action, activity, or method involving non-personal data, and asserting that no personal data is involved</t>
+  </si>
+  <si>
+    <t>Use of personal data within NonPersonalDataProcess should be considered a violation of the explicit constraint that no personal data is involved.</t>
+  </si>
+  <si>
+    <t>AIProcess</t>
+  </si>
+  <si>
+    <t>AI Process</t>
+  </si>
+  <si>
+    <t>An action, activity, or method involving AI technologies</t>
+  </si>
+  <si>
+    <t>EDITORIAL: move this to AI extension?</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>ParentProperty</t>
+  </si>
+  <si>
+    <t>CreationDate</t>
+  </si>
+  <si>
+    <t>hasPersonalDataHandling</t>
+  </si>
+  <si>
+    <t>has personal data handling</t>
+  </si>
+  <si>
+    <t>Indicates association with Personal Data Handling</t>
+  </si>
+  <si>
+    <t>dpv:Relation</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P Krog</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/community/dpvcg/wiki/MinutesOfMeeting_20220119</t>
+  </si>
+  <si>
+    <t>hasProcess</t>
+  </si>
+  <si>
+    <t>has process</t>
+  </si>
+  <si>
+    <t>Indicates association with a Process</t>
+  </si>
+  <si>
+    <t>hasPersonalDataProcess</t>
+  </si>
+  <si>
+    <t>has personal data process</t>
+  </si>
+  <si>
+    <t>Indicates association with a Personal Data Process</t>
+  </si>
+  <si>
     <t>dpv:PersonalDataProcess</t>
   </si>
   <si>
-    <t>Personal Data Process</t>
-  </si>
-  <si>
-    <t>An action, activity, or method involving personal data</t>
+    <t>hasNonPersonalDataProcess</t>
+  </si>
+  <si>
+    <t>has non-personal data process</t>
+  </si>
+  <si>
+    <t>Indicates association with a Non-Personal Data Process</t>
   </si>
   <si>
     <t>dpv:NonPersonalDataProcess</t>
   </si>
   <si>
-    <t>Non-Personal Data Process</t>
-  </si>
-  <si>
-    <t>An action, activity, or method involving non-personal data, and asserting that no personal data is involved</t>
-  </si>
-  <si>
-    <t>Use of personal data within NonPersonalDataProcess should be considered a violation of the explicit constraint that no personal data is involved.</t>
+    <t>hasAIProcess</t>
+  </si>
+  <si>
+    <t>has AI process</t>
+  </si>
+  <si>
+    <t>Indicates association with a AI Process</t>
   </si>
   <si>
     <t>dpv:AIProcess</t>
-  </si>
-  <si>
-    <t>AI Process</t>
-  </si>
-  <si>
-    <t>An action, activity, or method involving AI technologies</t>
-  </si>
-  <si>
-    <t>EDITORIAL: move this to AI extension?</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>ParentProperty</t>
-  </si>
-  <si>
-    <t>CreationDate</t>
-  </si>
-  <si>
-    <t>hasPersonalDataHandling</t>
-  </si>
-  <si>
-    <t>has personal data handling</t>
-  </si>
-  <si>
-    <t>Indicates association with Personal Data Handling</t>
-  </si>
-  <si>
-    <t>dpv:Relation</t>
-  </si>
-  <si>
-    <t>Harshvardhan J. Pandit, Georg P Krog</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/community/dpvcg/wiki/MinutesOfMeeting_20220119</t>
-  </si>
-  <si>
-    <t>hasProcess</t>
-  </si>
-  <si>
-    <t>has process</t>
-  </si>
-  <si>
-    <t>Indicates association with a Process</t>
-  </si>
-  <si>
-    <t>hasPersonalDataProcess</t>
-  </si>
-  <si>
-    <t>has personal data process</t>
-  </si>
-  <si>
-    <t>Indicates association with a Personal Data Process</t>
-  </si>
-  <si>
-    <t>hasNonPersonalDataProcess</t>
-  </si>
-  <si>
-    <t>has non-personal data process</t>
-  </si>
-  <si>
-    <t>Indicates association with a Non-Personal Data Process</t>
-  </si>
-  <si>
-    <t>hasAIProcess</t>
-  </si>
-  <si>
-    <t>has AI process</t>
-  </si>
-  <si>
-    <t>Indicates association with a AI Process</t>
   </si>
   <si>
     <t>EDITORIAL: Move to AI Extension?</t>
@@ -2935,7 +2944,7 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>214</v>
@@ -6224,7 +6233,7 @@
         <v>216</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>238</v>
@@ -6260,19 +6269,19 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>216</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>238</v>
@@ -6308,19 +6317,19 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>216</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>238</v>
@@ -6328,7 +6337,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
       <c r="I6" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J6" s="35"/>
       <c r="K6" s="8">
@@ -6382,43 +6391,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C15" s="37"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C16" s="37"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" s="37"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C21" s="37"/>
     </row>

</xml_diff>